<commit_message>
removed duty cycle warning from PROD and PROD-TEST testing sheets
</commit_message>
<xml_diff>
--- a/scripts/codemagic-ci/testing/PR-Test-Plan-Template-Android-QA.xlsx
+++ b/scripts/codemagic-ci/testing/PR-Test-Plan-Template-Android-QA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbryant/UCSD/campusmobile/scripts/codemagic-ci/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="13_ncr:1_{24687699-AA8E-BD41-9C89-3AB04E7A76E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DB1044C-09D4-41E5-B425-F39A029B6F11}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{24687699-AA8E-BD41-9C89-3AB04E7A76E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A914F4D-91D7-4752-874A-5C8AE6FD8718}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,7 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -540,12 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1025,7 +1019,7 @@
   <dimension ref="A1:U947"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="128" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="18" customHeight="1"/>
@@ -1418,8 +1412,8 @@
         <v>32</v>
       </c>
       <c r="B15" s="26"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="32" t="s">
+      <c r="C15" s="17"/>
+      <c r="D15" s="30" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="4"/>
@@ -1472,8 +1466,8 @@
         <v>36</v>
       </c>
       <c r="B17" s="25"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32" t="s">
+      <c r="C17" s="17"/>
+      <c r="D17" s="30" t="s">
         <v>37</v>
       </c>
       <c r="E17" s="19"/>
@@ -1511,8 +1505,8 @@
       <c r="U18" s="11"/>
     </row>
     <row r="19" spans="1:21" ht="18" customHeight="1">
-      <c r="C19" s="31"/>
-      <c r="D19" s="32" t="s">
+      <c r="C19" s="17"/>
+      <c r="D19" s="30" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="11"/>
@@ -1557,8 +1551,8 @@
       <c r="U20" s="11"/>
     </row>
     <row r="21" spans="1:21" ht="18" customHeight="1">
-      <c r="C21" s="31"/>
-      <c r="D21" s="32" t="s">
+      <c r="C21" s="17"/>
+      <c r="D21" s="30" t="s">
         <v>41</v>
       </c>
       <c r="E21" s="11"/>
@@ -1607,8 +1601,8 @@
         <v>43</v>
       </c>
       <c r="B23" s="25"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="32" t="s">
+      <c r="C23" s="17"/>
+      <c r="D23" s="30" t="s">
         <v>44</v>
       </c>
       <c r="F23" s="11"/>
@@ -1629,7 +1623,7 @@
       <c r="U23" s="11"/>
     </row>
     <row r="24" spans="1:21" ht="18" customHeight="1">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="31" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="17"/>
@@ -1657,7 +1651,7 @@
       </c>
       <c r="B25" s="26"/>
       <c r="C25" s="17"/>
-      <c r="D25" s="30"/>
+      <c r="D25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -22896,21 +22890,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5D778AC6A79A84EAA5B25C5A2BFF7B6" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4061397ea8fd8f272d8b26ba942e61d2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cd0eaed-44fe-4f97-8632-c05a782ebbb7" xmlns:ns3="75164c79-2692-43d6-94a7-34b44bf80abd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b13378bff9c1c8ba474ff50185c4976f" ns2:_="" ns3:_="">
     <xsd:import namespace="3cd0eaed-44fe-4f97-8632-c05a782ebbb7"/>
@@ -23075,8 +23054,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F9D8340-318B-43DD-BE9C-C876AB21B0D8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55915E3D-8D32-4904-AE11-02FF4B35B651}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23084,5 +23078,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55915E3D-8D32-4904-AE11-02FF4B35B651}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F9D8340-318B-43DD-BE9C-C876AB21B0D8}"/>
 </file>
</xml_diff>